<commit_message>
update .xsls file for byte unit
</commit_message>
<xml_diff>
--- a/byte_unit/docs/pbl_milik.xlsx
+++ b/byte_unit/docs/pbl_milik.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14775" activeTab="1"/>
+    <workbookView windowHeight="17355" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="IO listing" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="140">
   <si>
     <t>idx</t>
   </si>
@@ -87,81 +87,43 @@
     </r>
   </si>
   <si>
-    <t>sema_ready_i</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">semaphore signalling bit cpu unit is ready (if driven to '1) to take over data driven on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sema_data_out</t>
-    </r>
-  </si>
-  <si>
-    <t>sema_valid_o</t>
+    <t>sema_valid_i</t>
+  </si>
+  <si>
+    <t>signalling data written from bit to byte unit is valid</t>
+  </si>
+  <si>
+    <t>sema_data_i</t>
+  </si>
+  <si>
+    <t>data from bit to byte unit</t>
+  </si>
+  <si>
+    <t>sema_ready_o</t>
   </si>
   <si>
     <t>output</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">semaphore signalling data output to </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sema_data_out</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> port is valid for reading (if driven to '1')</t>
-    </r>
-  </si>
-  <si>
-    <t>sema_data_i</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data output by bit cpu unit to semaphore memory unit </t>
+    <t>signalling byte unit is not busy with recent sema operation anymore</t>
+  </si>
+  <si>
+    <t>sema_is_empty_i</t>
+  </si>
+  <si>
+    <t>signalling, that semaphore memory is empty (ready for another write)</t>
+  </si>
+  <si>
+    <t>sema_write_o</t>
+  </si>
+  <si>
+    <t>signalling data is to be written from byte to bit unit</t>
   </si>
   <si>
     <t>sema_data_o</t>
   </si>
   <si>
-    <t>data output by byte cpu unit to semaphore memory unit as a result of semaphore memory write instruction executed from program memory</t>
+    <t>data from byte to bit unit</t>
   </si>
   <si>
     <t>instruction name</t>
@@ -503,16 +465,16 @@
     <t>opcode width:</t>
   </si>
   <si>
-    <t>reg_id width (rs1_id, rs2_id, rd_id):</t>
+    <t>reg_id width (16 regs -- rs1_id, rs2_id, rd_id):</t>
   </si>
   <si>
     <t>reg width (rs1, rs2, rd):</t>
   </si>
   <si>
-    <t>reg operational width (how many bits of reg are used in arithmetic operations):</t>
-  </si>
-  <si>
-    <t>immediate value width (8 LSB operational, 8 MSB == 0):</t>
+    <t>reg operational width (16 for div/mul):</t>
+  </si>
+  <si>
+    <t>immediate value width (8 MSB == 0, 8 LSB operational):</t>
   </si>
 </sst>
 </file>
@@ -520,10 +482,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -569,8 +531,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -585,6 +556,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
@@ -592,7 +570,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
@@ -604,6 +590,43 @@
       <color theme="3"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -621,67 +644,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -692,7 +654,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -727,181 +689,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,17 +895,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -953,6 +921,41 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -986,183 +989,142 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="31" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1175,7 +1137,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1193,6 +1155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1533,13 +1496,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="4"/>
   <cols>
     <col min="2" max="2" width="17.3666666666667" customWidth="1"/>
     <col min="3" max="4" width="10.8166666666667" customWidth="1"/>
@@ -1625,13 +1588,13 @@
         <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D6" s="8">
         <v>1</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1640,10 +1603,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>6</v>
       </c>
       <c r="D7" s="8">
         <v>1</v>
@@ -1661,13 +1624,49 @@
         <v>17</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="8">
+        <f>A8+1</f>
+        <v>7</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="10">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8">
+        <f>A9+1</f>
+        <v>8</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1682,7 +1681,7 @@
   <dimension ref="A2:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="5"/>
@@ -1699,16 +1698,16 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1716,19 +1715,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1737,40 +1736,40 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <f t="shared" ref="A5:A32" si="0">A4+1</f>
+        <f t="shared" ref="A5:A34" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1779,19 +1778,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1800,19 +1799,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1821,19 +1820,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1842,19 +1841,19 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E9" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1863,19 +1862,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1884,19 +1883,19 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1905,19 +1904,19 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="F12" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1926,19 +1925,19 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1947,19 +1946,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1968,19 +1967,19 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1989,19 +1988,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C16" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="F16" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2010,19 +2009,19 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2031,19 +2030,19 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2052,19 +2051,19 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D19" s="2">
         <v>10000</v>
       </c>
       <c r="E19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2073,19 +2072,19 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D20" s="2">
         <v>10001</v>
       </c>
       <c r="E20" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2094,19 +2093,19 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="D21" s="2">
         <v>10010</v>
       </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="F21" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2115,19 +2114,19 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2">
         <v>10011</v>
       </c>
       <c r="E22" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="F22" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2136,19 +2135,19 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E23" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="F23" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2157,19 +2156,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="E24" t="s">
-        <v>92</v>
-      </c>
-      <c r="F24" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -2178,19 +2177,19 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E25" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F25" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2199,19 +2198,19 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="E26" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="F26" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2220,19 +2219,19 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
         <v>101</v>
       </c>
-      <c r="C27" t="s">
-        <v>97</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E27" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F27" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2241,19 +2240,19 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" t="s">
         <v>104</v>
-      </c>
-      <c r="C28" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E28" t="s">
-        <v>106</v>
-      </c>
-      <c r="F28" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2262,19 +2261,19 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C29" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F29" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2283,19 +2282,19 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E30" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F30" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2304,82 +2303,82 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="C31" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E31" t="s">
+        <v>122</v>
+      </c>
+      <c r="F31" t="s">
         <v>118</v>
-      </c>
-      <c r="F31" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <f>A31+1</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C32" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E32" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <f>A32+1</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F33" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <f>A33+1</f>
+        <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="C34" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="F34" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="4:4">
@@ -2404,7 +2403,7 @@
     </row>
     <row r="41" spans="5:6">
       <c r="E41" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="F41">
         <v>21</v>
@@ -2412,7 +2411,7 @@
     </row>
     <row r="42" spans="5:6">
       <c r="E42" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="F42">
         <v>5</v>
@@ -2420,7 +2419,7 @@
     </row>
     <row r="43" spans="5:6">
       <c r="E43" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="F43">
         <v>4</v>
@@ -2428,7 +2427,7 @@
     </row>
     <row r="44" spans="5:6">
       <c r="E44" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="F44">
         <v>16</v>
@@ -2436,7 +2435,7 @@
     </row>
     <row r="45" spans="5:6">
       <c r="E45" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="F45">
         <v>8</v>
@@ -2444,7 +2443,7 @@
     </row>
     <row r="46" spans="5:6">
       <c r="E46" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F46">
         <v>16</v>

</xml_diff>